<commit_message>
fix the bugs in kurtosis
</commit_message>
<xml_diff>
--- a/csv/1stRound/h3k4me3/h3k4me3_total_width_TSSdownstream_grid_change.xlsx
+++ b/csv/1stRound/h3k4me3/h3k4me3_total_width_TSSdownstream_grid_change.xlsx
@@ -87,7 +87,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.148565429321335"/>
+          <c:y val="0.0320197044334975"/>
+          <c:w val="0.785351331083614"/>
+          <c:h val="0.84889996509057"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -109,7 +119,21 @@
             <a:ln w="47625">
               <a:noFill/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>h3k4me3_total_width_window_grid!$A$2:$A$43</c:f>
@@ -384,45 +408,95 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2008725720"/>
-        <c:axId val="-2009060408"/>
+        <c:axId val="-2079602952"/>
+        <c:axId val="-2080121304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2008725720"/>
+        <c:axId val="-2079602952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="50000.0"/>
-          <c:min val="-50000.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relative distance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> to TSS (kb)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2009060408"/>
+        <c:crossAx val="-2080121304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:builtInUnit val="thousands"/>
-          <c:dispUnitsLbl>
-            <c:layout/>
-          </c:dispUnitsLbl>
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2009060408"/>
+        <c:axId val="-2080121304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Best</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> negative logP</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0533273340832396"/>
+              <c:y val="0.357687638183158"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2008725720"/>
-        <c:crossesAt val="-50000.0"/>
+        <c:crossAx val="-2079602952"/>
+        <c:crossesAt val="-250000.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>

</xml_diff>